<commit_message>
adjusted height and width size
</commit_message>
<xml_diff>
--- a/demo/src/main/resources/spreadsheet/Workout Spreadsheet.xlsx
+++ b/demo/src/main/resources/spreadsheet/Workout Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\keonv\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{915D8E89-5C5C-4696-BB95-1AE3CFA09D01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46D030BA-1D2C-4F96-8BD1-E3FFDB98EDAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,17 +16,6 @@
     <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -828,265 +817,265 @@
     <t>smith_machine_close_grip_bench_press.jpg</t>
   </si>
   <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/CjHIKDQ4RQo?si=Nl6wuK6-gTj95SLa" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/O5viuEPDXKY?si=cSxtgvqbGxYsbXY7&amp;amp;start=95" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/AduT4Eq-iP0?si=5QgVZZjgmXXFKdlX" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/p5dCqF7wWUw?si=Nwl1mW5y0PJX0mVs" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/sqNwDkUU_Ps?si=ffMH9200TlKy9X0e" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/NwwDBARCGgo?si=GZvpvwFMZUwBBC4o" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/HxsFneJFM2c?si=dnBxdpkz3fTVilkU" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/yISC2qwdh9I?si=Gv04SZL6mtskKWsO" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/XugMoMDxyhM?si=bKcqHyNzFUsOHZjz&amp;amp;start=7" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/6_eLpWiNijE?si=3fSWhUhdacTJccyt" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/r58nxtqD_zQ?si=vd5gszhObAJVGBaR&amp;amp;start=7" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/KC-ZSfOmXgE?si=M9sBWmUvKlb0HQKU&amp;amp;start=7" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/9Gf-Ourup_k?si=WGxFVp_UH2LpfQoC" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/DMo3HJoawrU?si=F6EwklDWr_ONIrrg" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/3QcJggd_L24?si=1USxw-mpDTmiqWhe&amp;amp;start=95" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/l5qelXL5nfs?si=9o6AXZIgh94U9rRh&amp;amp;start=7" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/eGjt4lk6g34?si=9ToRIovqSG154x3m" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/Nhvz9EzdJ4U?si=_aDy1DSu928Gq2f2" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/4mfLHnFL0Uw?si=PAvgSkAmyw7vakXf" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/TnhIyp4kmO8?si=0uMxho43AHhjqXzX" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/aI2hGzsAMXs?si=NipUUIO78sUzGaL5" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/OLqZDUUD2b0?si=sHuJcbyAbI-NRGAZ&amp;amp;start=95" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/z-kOn7flIZg?si=T6X66IraESeO__8V" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/Z5FA9aq3L6A?si=Cc53pYHfvoolsi3A" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/MtXdEcW3Eog?si=53BHIkx_-yjPhqZE" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/GNlopToAZyg?si=DI0GDl97boWWVAHN" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/9wxRhONFsRA?si=zteT7mBh6I4NYSXr" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/m_UlDFNX4mk?si=AD50-IPsMZefHJ2v" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/hf7jnF45N_I?si=yR1gX7QSlGEcegmK" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/zkP0MsTcIVU?si=fdc4vxkfWo8tV5Os" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/SX1FE0URdv8?si=2y0VFuqw2Qn822lI" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/larn3Asl6oM?si=JkgOKUuFEWn-oqps" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/B4RznoFvTl4?si=1ofOg0sTJTqmxfqv" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/llD6MImgqe8?si=Qufg_OplNBKVu9Q3" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/9gglI77Kzq8?si=I2TrCEkoe4zoEDVq" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/NcDtORTfVNQ?si=p_hZabDe2QDEbOEN&amp;amp;start=95" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/qY7Yo0x5mhE?si=tYMu8SfmEsYsBTlR&amp;amp;start=95" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/UFStLR88gOk?si=mYlNRAKsMnEHhdzL" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/plb5jEO4Unw?si=toLkXql3nBT_X6_Y" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/NBR6tozmx2I?si=ccWPZioBHxZbpxHD&amp;amp;start=7" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/DxUNi119Qzs?si=CosuKkAF90KR3bv3" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/yPqv3ejnZvc?si=-Y7Eczr6k7O4MMfZ" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/p6KK6yHxd4k?si=_mEghTdVvpaQDV-r" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/vLuhN_glFZ8?si=mYolItied7OfsFrI" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/FShbaqrGGu4?si=tJZunZsRLOPhWYs3" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/0V-8kqnPPeM?si=hHCIrEwtG6FnCavk&amp;amp;start=7" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/yHzVcjDQKQU?si=LdtlPKxPjIEj0YiA&amp;amp;start=7" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/wsbcev7aYeU?si=kVqwaRd826S2wIgA" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/dL9ZzqtQI5c?si=A9Q81o6ik034YN6L" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/iXu2QK049rU?si=NtJLzj_YLpYPk0EE" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/JGeRYIZdojU?si=maAz1BsN9hpw3SL0" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/gcGNypjIQDo?si=pKG6e4kD5O3nw1ji&amp;amp;start=7" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/tAJucO55-bQ?si=WyAeUzYhX4uHS0HU" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/-eO_VydErV0?si=Epzsslcfk6pyfmSV&amp;amp;start=95" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/zBV3ceGyAxw?si=ETmktI93Xs0IjutC" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/kVWtlBl5PvU?si=hgPb3uj_R1sFhrxR&amp;amp;start=7" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/QJ4T1pUJ_zw?si=VhSRMkAqqHTI4moj&amp;amp;start=7" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/-5MmFTKLC-0?si=bvM5E-fc2nXCawJj" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/oYbWXyEdQkQ?si=WwJoVuxkv51_lIZ-" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/N5x5M1x1Gd0?si=qDKEbauv_AEUtelO" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/aweBS7K71l8?si=vAuxTf3OMzYa7OLu" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/s6u3ESE4kMg?si=bc8LUSSMVXb3pGtZ&amp;amp;start=7" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/hh5516HCu4k?si=5GMEeDZ_gBHFJK0i&amp;amp;start=95" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/Ex81dYhX8FI?si=cevws9c_XZRvJUNM&amp;amp;start=95" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/leEtTkR_OKE?si=eOnUs0h1V0XZlV_Y&amp;amp;start=7" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/nWyx81AfTos?si=AvMUK_qtTY3AZeq6" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/wUbsMNkkpLk?si=sQi9auOabwGGJdif" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/FiVuO6Y5UcU?si=H_zDCl3k_YPZWdgU&amp;amp;start=7" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/wFj808u2HWU?si=LhhnwtHFJTbDd1Hz&amp;amp;start=7" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/qca__Qgjf1Y?si=D3QoC_THyNq1Tobf&amp;amp;start=7" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/4ZDm5EbiFI8?si=8NpQ2a_UAKSFW9j1" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/6A0yJetx7hg?si=8ZiirLUBSFq_NNxG" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/gjr-QAdsq4o?si=6x55ZDRioY_CyVZL&amp;amp;start=7" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/xZyGP55NkAo?si=gx_uCYNdTmNugUop" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/DMrxbUgoZTg?si=IQER0HKK1FE6bf2E" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/MSSEoBnxPtM?si=r5d2kWtONjHbWf0w&amp;amp;start=7" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/-cqo-oailwk?si=yh977tkDtEt_cle0" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/scs5XcsZuc8?si=jOPbgwy0P-0qWeQz" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/Ja6ZlIDONac?si=Vg55qjjgge4WA8eK&amp;amp;start=7" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/TeFo51Q_Nsc?si=LpIE1CYbN7N0e7He" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/lJoozxC0Rns?si=YPLIRQLrrg8J6wnZ" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/LXkCrxn3caQ?si=IMMWUdq3W9txtm8B" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/SqO-VUEak2M?si=yQh_sJU0qqjsdmlw" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/b9FJ4hIK3pI?si=9auJRLdRYifV6rg_&amp;amp;start=7" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/-0N2xTi69t8?si=gN9p4MOoVdgIKxaq&amp;amp;start=7" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/CjAVezAggkI?si=_LrPszihHlwmBPKb" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;iframe width="100%" height="100%" src="https://www.youtube.com/embed/qf_FTh3QyYs?si=vAlffNIQgYRWeK3Z&amp;amp;start=95" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/CjHIKDQ4RQo?si=Nl6wuK6-gTj95SLa" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/AduT4Eq-iP0?si=5QgVZZjgmXXFKdlX" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/O5viuEPDXKY?si=cSxtgvqbGxYsbXY7&amp;amp;start=95" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/p5dCqF7wWUw?si=Nwl1mW5y0PJX0mVs" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/sqNwDkUU_Ps?si=ffMH9200TlKy9X0e" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/HxsFneJFM2c?si=dnBxdpkz3fTVilkU" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/NwwDBARCGgo?si=GZvpvwFMZUwBBC4o" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/yISC2qwdh9I?si=Gv04SZL6mtskKWsO" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/XugMoMDxyhM?si=bKcqHyNzFUsOHZjz&amp;amp;start=7" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/6_eLpWiNijE?si=3fSWhUhdacTJccyt" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/r58nxtqD_zQ?si=vd5gszhObAJVGBaR&amp;amp;start=7" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/KC-ZSfOmXgE?si=M9sBWmUvKlb0HQKU&amp;amp;start=7" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/DMo3HJoawrU?si=F6EwklDWr_ONIrrg" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/9Gf-Ourup_k?si=WGxFVp_UH2LpfQoC" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/3QcJggd_L24?si=1USxw-mpDTmiqWhe&amp;amp;start=95" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/l5qelXL5nfs?si=9o6AXZIgh94U9rRh&amp;amp;start=7" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/eGjt4lk6g34?si=9ToRIovqSG154x3m" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/Nhvz9EzdJ4U?si=_aDy1DSu928Gq2f2" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/4mfLHnFL0Uw?si=PAvgSkAmyw7vakXf" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/TnhIyp4kmO8?si=0uMxho43AHhjqXzX" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/aI2hGzsAMXs?si=NipUUIO78sUzGaL5" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/OLqZDUUD2b0?si=sHuJcbyAbI-NRGAZ&amp;amp;start=95" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/z-kOn7flIZg?si=T6X66IraESeO__8V" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/Z5FA9aq3L6A?si=Cc53pYHfvoolsi3A" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/MtXdEcW3Eog?si=53BHIkx_-yjPhqZE" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/GNlopToAZyg?si=DI0GDl97boWWVAHN" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/9wxRhONFsRA?si=zteT7mBh6I4NYSXr" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/m_UlDFNX4mk?si=AD50-IPsMZefHJ2v" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/hf7jnF45N_I?si=yR1gX7QSlGEcegmK" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/zkP0MsTcIVU?si=fdc4vxkfWo8tV5Os" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/SX1FE0URdv8?si=2y0VFuqw2Qn822lI" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/larn3Asl6oM?si=JkgOKUuFEWn-oqps" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/B4RznoFvTl4?si=1ofOg0sTJTqmxfqv" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/llD6MImgqe8?si=Qufg_OplNBKVu9Q3" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/9gglI77Kzq8?si=I2TrCEkoe4zoEDVq" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/NcDtORTfVNQ?si=p_hZabDe2QDEbOEN&amp;amp;start=95" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/qY7Yo0x5mhE?si=tYMu8SfmEsYsBTlR&amp;amp;start=95" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/UFStLR88gOk?si=mYlNRAKsMnEHhdzL" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/plb5jEO4Unw?si=toLkXql3nBT_X6_Y" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/NBR6tozmx2I?si=ccWPZioBHxZbpxHD&amp;amp;start=7" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/DxUNi119Qzs?si=CosuKkAF90KR3bv3" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/yPqv3ejnZvc?si=-Y7Eczr6k7O4MMfZ" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/p6KK6yHxd4k?si=_mEghTdVvpaQDV-r" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/vLuhN_glFZ8?si=mYolItied7OfsFrI" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/FShbaqrGGu4?si=tJZunZsRLOPhWYs3" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/0V-8kqnPPeM?si=hHCIrEwtG6FnCavk&amp;amp;start=7" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/wsbcev7aYeU?si=kVqwaRd826S2wIgA" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/yHzVcjDQKQU?si=LdtlPKxPjIEj0YiA&amp;amp;start=7" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/gcGNypjIQDo?si=pKG6e4kD5O3nw1ji&amp;amp;start=7" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/dL9ZzqtQI5c?si=A9Q81o6ik034YN6L" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/iXu2QK049rU?si=NtJLzj_YLpYPk0EE" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/JGeRYIZdojU?si=maAz1BsN9hpw3SL0" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/tAJucO55-bQ?si=WyAeUzYhX4uHS0HU" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/-eO_VydErV0?si=Epzsslcfk6pyfmSV&amp;amp;start=95" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/zBV3ceGyAxw?si=ETmktI93Xs0IjutC" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/kVWtlBl5PvU?si=hgPb3uj_R1sFhrxR&amp;amp;start=7" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/QJ4T1pUJ_zw?si=VhSRMkAqqHTI4moj&amp;amp;start=7" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/-5MmFTKLC-0?si=bvM5E-fc2nXCawJj" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/oYbWXyEdQkQ?si=WwJoVuxkv51_lIZ-" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/N5x5M1x1Gd0?si=qDKEbauv_AEUtelO" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/aweBS7K71l8?si=vAuxTf3OMzYa7OLu" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/s6u3ESE4kMg?si=bc8LUSSMVXb3pGtZ&amp;amp;start=7" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/hh5516HCu4k?si=5GMEeDZ_gBHFJK0i&amp;amp;start=95" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/Ex81dYhX8FI?si=cevws9c_XZRvJUNM&amp;amp;start=95" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/wUbsMNkkpLk?si=sQi9auOabwGGJdif" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/nWyx81AfTos?si=AvMUK_qtTY3AZeq6" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/leEtTkR_OKE?si=eOnUs0h1V0XZlV_Y&amp;amp;start=7" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/FiVuO6Y5UcU?si=H_zDCl3k_YPZWdgU&amp;amp;start=7" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/wFj808u2HWU?si=LhhnwtHFJTbDd1Hz&amp;amp;start=7" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/qca__Qgjf1Y?si=D3QoC_THyNq1Tobf&amp;amp;start=7" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/4ZDm5EbiFI8?si=8NpQ2a_UAKSFW9j1" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/6A0yJetx7hg?si=8ZiirLUBSFq_NNxG" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/gjr-QAdsq4o?si=6x55ZDRioY_CyVZL&amp;amp;start=7" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/xZyGP55NkAo?si=gx_uCYNdTmNugUop" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/DMrxbUgoZTg?si=IQER0HKK1FE6bf2E" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/MSSEoBnxPtM?si=r5d2kWtONjHbWf0w&amp;amp;start=7" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/-cqo-oailwk?si=yh977tkDtEt_cle0" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/scs5XcsZuc8?si=jOPbgwy0P-0qWeQz" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/Ja6ZlIDONac?si=Vg55qjjgge4WA8eK&amp;amp;start=7" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/TeFo51Q_Nsc?si=LpIE1CYbN7N0e7He" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/lJoozxC0Rns?si=YPLIRQLrrg8J6wnZ" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/LXkCrxn3caQ?si=IMMWUdq3W9txtm8B" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/SqO-VUEak2M?si=yQh_sJU0qqjsdmlw" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/b9FJ4hIK3pI?si=9auJRLdRYifV6rg_&amp;amp;start=7" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/-0N2xTi69t8?si=gN9p4MOoVdgIKxaq&amp;amp;start=7" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/CjAVezAggkI?si=_LrPszihHlwmBPKb" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="960" height="720" src="https://www.youtube.com/embed/qf_FTh3QyYs?si=vAlffNIQgYRWeK3Z&amp;amp;start=95" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
   </si>
 </sst>
 </file>
@@ -1866,9 +1855,9 @@
   </sheetPr>
   <dimension ref="A1:O90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="O90" sqref="O90"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="N103" sqref="N103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -2025,7 +2014,7 @@
         <v>22</v>
       </c>
       <c r="O3" s="32" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="15.75" customHeight="1" thickBot="1">
@@ -2072,7 +2061,7 @@
         <v>25</v>
       </c>
       <c r="O4" s="32" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.75" customHeight="1" thickBot="1">
@@ -2213,7 +2202,7 @@
         <v>37</v>
       </c>
       <c r="O7" s="32" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75" customHeight="1" thickBot="1">
@@ -2260,7 +2249,7 @@
         <v>40</v>
       </c>
       <c r="O8" s="32" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="15.75" customHeight="1" thickBot="1">
@@ -2542,7 +2531,7 @@
         <v>59</v>
       </c>
       <c r="O14" s="32" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="15.75" customHeight="1" thickBot="1">
@@ -2589,7 +2578,7 @@
         <v>62</v>
       </c>
       <c r="O15" s="32" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="15.75" customHeight="1" thickBot="1">
@@ -4187,7 +4176,7 @@
         <v>154</v>
       </c>
       <c r="O49" s="32" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="50" spans="1:15" ht="15.75" customHeight="1" thickBot="1">
@@ -4234,7 +4223,7 @@
         <v>156</v>
       </c>
       <c r="O50" s="32" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="51" spans="1:15" ht="15.75" customHeight="1" thickBot="1">
@@ -4281,7 +4270,7 @@
         <v>158</v>
       </c>
       <c r="O51" s="32" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="52" spans="1:15" ht="15.75" customHeight="1" thickBot="1">
@@ -4328,7 +4317,7 @@
         <v>161</v>
       </c>
       <c r="O52" s="32" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="53" spans="1:15" ht="15.75" customHeight="1" thickBot="1">
@@ -4375,7 +4364,7 @@
         <v>164</v>
       </c>
       <c r="O53" s="32" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="54" spans="1:15" ht="15.75" customHeight="1" thickBot="1">
@@ -4422,7 +4411,7 @@
         <v>167</v>
       </c>
       <c r="O54" s="32" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="55" spans="1:15" ht="15.75" customHeight="1" thickBot="1">
@@ -5033,7 +5022,7 @@
         <v>200</v>
       </c>
       <c r="O67" s="32" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="68" spans="1:15" ht="15.75" customHeight="1" thickBot="1">
@@ -5127,7 +5116,7 @@
         <v>204</v>
       </c>
       <c r="O69" s="32" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
     </row>
     <row r="70" spans="1:15" ht="15.75" customHeight="1" thickBot="1">

</xml_diff>